<commit_message>
Biblia lida a partir das referencias
</commit_message>
<xml_diff>
--- a/criardataset/ojb/Kefa II.xlsx
+++ b/criardataset/ojb/Kefa II.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>Livro</t>
   </si>
@@ -43,114 +43,120 @@
     <t>Ibn</t>
   </si>
   <si>
+    <t>Onkelos</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Isaiah</t>
+  </si>
+  <si>
+    <t>Psalms</t>
+  </si>
+  <si>
     <t>Leviticus</t>
   </si>
   <si>
-    <t>Isaiah</t>
-  </si>
-  <si>
     <t>Numbers</t>
   </si>
   <si>
-    <t>Psalms</t>
+    <t>Genesis</t>
   </si>
   <si>
     <t>Proverbs</t>
   </si>
   <si>
-    <t>Genesis</t>
-  </si>
-  <si>
     <t>Daniel</t>
   </si>
   <si>
     <t>Exodus</t>
   </si>
   <si>
+    <t>42 Here is Avdi [Moshiach, see Zech 3:8., Isa 52:13], whom I uphold., Mine Bachir (Elect One, Chosen One), in whom My nefesh delighteth., I have put My Ruach [Hakodesh] upon Him., He [Moshiach] shall bring forth mishpat to the Goyim.</t>
+  </si>
+  <si>
+    <t>6 By the Devar Hashem were Shomayim made., and all the tz’va (host) of them by the ruach (breath) of His mouth [MJ 11:3., Yn 1:1., Psa 56:5].</t>
+  </si>
+  <si>
     <t>20 But whatsoever hath a mum, that shall ye not offer, for it shall not be for you leratzon (acceptable [before Hashem]).</t>
   </si>
   <si>
-    <t>42 Here is Avdi [Moshiach, see Zech 3:8., Isa 52:13], whom I uphold., Mine Bachir (Elect One, Chosen One), in whom My nefesh delighteth., I have put My Ruach [Hakodesh] upon Him., He [Moshiach] shall bring forth mishpat to the Goyim.</t>
+    <t>4 For an elef shanim in Thy sight are but as yom etmol (yesterday) when it is past, and as an ashmurah (watch, division of time) in the lailah.</t>
   </si>
   <si>
     <t>23 But if ye will not do so, hinei, ye have sinned against Hashem and be sure chattatechem (your sin) will find you out.</t>
   </si>
   <si>
-    <t>4 For an elef shanim in Thy sight are but as yom etmol (yesterday) when it is past, and as an ashmurah (watch, division of time) in the lailah.</t>
-  </si>
-  <si>
     <t>7 I will declare the chok (decree): Hashem hath said unto me, Thou art Beni (My Son, i.e. Ben HaElohim Moshiach)., HaYom (today) I have begotten thee.</t>
   </si>
   <si>
+    <t>17 I see him, but not now., I behold him, but not karov (near)., there shall come a Kokhav (Star, i.e. Moshiach, see Targums) out of Ya’akov, and a Shevet (Sceptre) shall rise out of Yisroel, and shall strike through the temples (i.e., sides of the head) of Moav, and destroy all the Bnei Shet.</t>
+  </si>
+  <si>
+    <t>2 And He said, Take now thy son, thine ben yachid (only son) Yitzchak, whom thou lovest, and get thee into eretz Moriah., and offer him there for a burnt offering upon one of the mountains which I will tell thee of.</t>
+  </si>
+  <si>
     <t>11 As a kelev returneth to his vomit, so a kesil (fool) returneth to his folly.</t>
   </si>
   <si>
+    <t>7 He was oppressed, and he was afflicted, yet he opened not his mouth., he is brought as a seh (lamb., see Shemot 12:3) to the slaughter, and as a sheep before her shearers is dumb, so he openeth not his mouth.</t>
+  </si>
+  <si>
     <t>9 And he made his kever (grave) with the resha’im, and with the oisher (rich man., see Mt 27:57-60) bemotayv (in his deaths, intensive plural should be translated singular, death)., because he had done no chamas (violence), neither was any mirmah (deceit) in his mouth. T.N. We stray as sheep., we return in Moshiach as children (zera)., the Techiyas HaMoshiach (Resurrection of Moshiach) predicted in v. 10 [Dead Sea Scrolls Isaiah Scroll says Moshiach "will see the light [of life].," see also the Targum HaShivim]</t>
   </si>
   <si>
-    <t>2 And He said, Take now thy son, thine ben yachid (only son) Yitzchak, whom thou lovest, and get thee into eretz Moriah., and offer him there for a burnt offering upon one of the mountains which I will tell thee of.</t>
+    <t>17 For, hinei, I create Shomayim Chadashim and eretz Chadashah., and the rishonot shall not be remembered, nor come into mind.</t>
   </si>
   <si>
     <t>24 Shivi’im heptads is decreed upon thy people and upon thy Ir Kodesh (Holy City), to restrain the peysha (transgression), and to make an end of chattat (sin), and to make kapporah for avon, and to bring in Tzedek Olamim (Everlasting Righteousness), and to seal up the chazon and navi, and to anoint the Kodesh HaKodashim.</t>
   </si>
   <si>
-    <t>6 By the Devar Hashem were Shomayim made., and all the tz’va (host) of them by the ruach (breath) of His mouth [MJ 11:3., Yn 1:1., Psa 56:5].</t>
-  </si>
-  <si>
-    <t>17 For, hinei, I create Shomayim Chadashim and eretz Chadashah., and the rishonot shall not be remembered, nor come into mind.</t>
-  </si>
-  <si>
-    <t>17 I see him, but not now., I behold him, but not karov (near)., there shall come a Kokhav (Star, i.e. Moshiach, see Targums) out of Ya’akov, and a Shevet (Sceptre) shall rise out of Yisroel, and shall strike through the temples (i.e., sides of the head) of Moav, and destroy all the Bnei Shet.</t>
-  </si>
-  <si>
     <t>5 Your seh (lamb [see Yeshayah 53:7]) shall be tamim (without blemish), a zachar (male) within its first year., ye shall take it out from the sheep, or from the goats.,</t>
   </si>
   <si>
-    <t>7 He was oppressed, and he was afflicted, yet he opened not his mouth., he is brought as a seh (lamb., see Shemot 12:3) to the slaughter, and as a sheep before her shearers is dumb, so he openeth not his mouth.</t>
+    <t>"Eis o meu servo, a quem sustento, o meu escolhido, em quem tenho prazer. Porei nele o meu Espírito, e ele trará justiça às nações.</t>
+  </si>
+  <si>
+    <t>Mediante a palavra do Senhor foram feitos os céus, e os corpos celestes, pelo sopro de sua boca.</t>
   </si>
   <si>
     <t>Não tragam nenhum animal defeituoso, porque não será aceito em favor de vocês.</t>
   </si>
   <si>
-    <t>"Eis o meu servo, a quem sustento, o meu escolhido, em quem tenho prazer. Porei nele o meu Espírito, e ele trará justiça às nações.</t>
+    <t>De fato, mil anos para ti são como o dia de ontem que passou, como as horas da noite.</t>
   </si>
   <si>
     <t>"Mas, se vocês não fizerem isso, estarão pecando contra o Senhor; e estejam certos de que vocês não escaparão do pecado que cometeram.</t>
   </si>
   <si>
-    <t>De fato, mil anos para ti são como o dia de ontem que passou, como as horas da noite.</t>
-  </si>
-  <si>
     <t>Proclamarei o decreto do Senhor: Ele me disse: "Tu és meu filho; eu hoje te gerei.</t>
   </si>
   <si>
+    <t>Eu o vejo, mas não agora; eu o avisto, mas não de perto. Uma estrela surgirá de Jacó; um cetro se levantará de Israel. Ele esmagará as frontes de Moabe e o crânio de todos os descendentes de Sete.</t>
+  </si>
+  <si>
+    <t>Então disse Deus: "Tome seu filho, seu único filho, Isaque, a quem você ama, e vá para a região de Moriá. Sacrifique-o ali como holocausto num dos montes que lhe indicarei".</t>
+  </si>
+  <si>
     <t>Como o cão volta ao seu vômito, assim o insensato repete a sua insensatez.</t>
   </si>
   <si>
+    <t>Ele foi oprimido e afligido, contudo não abriu a sua boca; como um cordeiro foi levado para o matadouro, e como uma ovelha que diante de seus tosquiadores fica calada, ele não abriu a sua boca.</t>
+  </si>
+  <si>
     <t>Foi-lhe dado um túmulo com os ímpios, e com os ricos em sua morte, embora não tivesse cometido qualquer violência nem houvesse qualquer mentira em sua boca.</t>
   </si>
   <si>
-    <t>Então disse Deus: "Tome seu filho, seu único filho, Isaque, a quem você ama, e vá para a região de Moriá. Sacrifique-o ali como holocausto num dos montes que lhe indicarei".</t>
+    <t>"Pois vejam! Criarei novos céus e nova terra, e as coisas passadas não serão lembradas. Jamais virão à mente!</t>
   </si>
   <si>
     <t>"Setenta semanas estão decretadas para o seu povo e sua santa cidade para acabar com a transgressão, para dar fim ao pecado, para expiar as culpas, para trazer justiça eterna, para cumprir a visão e a profecia, e para ungir o santíssimo.</t>
   </si>
   <si>
-    <t>Mediante a palavra do Senhor foram feitos os céus, e os corpos celestes, pelo sopro de sua boca.</t>
-  </si>
-  <si>
-    <t>"Pois vejam! Criarei novos céus e nova terra, e as coisas passadas não serão lembradas. Jamais virão à mente!</t>
-  </si>
-  <si>
-    <t>Eu o vejo, mas não agora; eu o avisto, mas não de perto. Uma estrela surgirá de Jacó; um cetro se levantará de Israel. Ele esmagará as frontes de Moabe e o crânio de todos os descendentes de Sete.</t>
-  </si>
-  <si>
     <t>O animal escolhido será macho de um ano, sem defeito, e pode ser cordeiro ou cabrito.</t>
   </si>
   <si>
-    <t>Ele foi oprimido e afligido, contudo não abriu a sua boca; como um cordeiro foi levado para o matadouro, e como uma ovelha que diante de seus tosquiadores fica calada, ele não abriu a sua boca.</t>
-  </si>
-  <si>
     <t>'&lt;b&gt;Behold My servant, I will support him&lt;/b&gt; Behold My servant Jacob is not like you, for I will support him.', '&lt;b&gt;My chosen one&lt;/b&gt; Israel is called ‘My chosen one’ ([mss.:] His chosen one) (&lt;a class ="refLink" href="/Psalms.135.4" data-ref="Psalms 135:4"&gt;Ps. 135:4&lt;/a&gt;) “For the Eternal chose Jacob for Himself.” Scripture states also (infra 45:4): “For the sake of My servant Jacob and Israel My chosen one.”', '&lt;b&gt;whom My soul desires; I have placed My spirit upon him&lt;/b&gt; to let his prophets know My secret, and his end will be that ‘he shall promulgate justice to the nations,’ as it is stated (supra 2:3): “And let Him teach us of His ways etc.”'</t>
   </si>
   <si>
@@ -160,30 +166,30 @@
     <t>'&lt;b&gt;I will tell of the decree&lt;/b&gt; Said David, “This is an established decree, and [one] that I have received to tell this and to make known.”', '&lt;b&gt;The Lord said to me&lt;/b&gt; through Nathan, Gad, and Samuel.', '&lt;b&gt;You are My son&lt;/b&gt; The head over Israel, who are called “My firstborn son.” And they will endure through you, as is stated concerning Abner (&lt;a class ="refLink" href="/II_Samuel.3.18" data-ref="II Samuel 3:18"&gt;II Sam. 3:18&lt;/a&gt;): “for God said, etc., ‘By the hand of My bondsman David shall I deliver...Israel.’” And for their sake, you are before Me as a son because they are all dependent upon you.', '&lt;b&gt;this day have I&lt;/b&gt; for I have enthroned you over them.', '&lt;b&gt;begotten you&lt;/b&gt; to be called My son and to be beloved to Me as a son for their sake, as it is stated (&lt;a class ="refLink" href="/II_Samuel.7.14" data-ref="II Samuel 7:14"&gt;II Sam. 7:14&lt;/a&gt;) concerning Solomon: “I will be to him a father, and he shall be to Me a son.” We find further concerning David (&lt;a class ="refLink" href="/Psalms.89.27" data-ref="Psalms 89:27"&gt;Ps. 89:27&lt;/a&gt;) “He shall call Me, ‘You are my Father, my God, and the Rock of my salvation.’”'</t>
   </si>
   <si>
+    <t>'אראנו I SEE HIM — I see the preeminence of Jacob and his greatness, but it is not now (ולא עתה), but will be after some time.', 'דרך כוכב A STAR COMETH OUT [OF JACOB] — Understand this as the Targum does (“a king will arise from Jacob”). The word דרך has the same meaning as in (&lt;a class ="refLink" href="/Lamentations.2.4" data-ref="Lamentations 2:4"&gt;Lamentations 2:4&lt;/a&gt;): “He has bent (דרך lit., trodden) his bow; this expression is used because the star shoots across [the heavens] as an arrow does when the bow is trodden. In O. F. destent. It is as much as to say, “Prosperity (a good fortune) will rise”.', 'וקם שבט AND A שבט RISES [OUT OF ISRAEL] — a king, who chastises with the rod (שבט) and has sovereign power.', 'ומחץ פאתי מואב AND PIERCETH THE CORNERS OF MOAB — This is a reference to David of whom it is stated, (&lt;a class ="refLink" href="/II_Samuel.8.2" data-ref="II Samuel 8:2"&gt;II Samuel 8:2&lt;/a&gt;) “[And he smote Moab] … making them to lie down on the ground and he measured two lines to put to death etc.”.', 'וקרקר AND UNDERMINETH — This is an expression denoting “digging”, as in (&lt;a class ="refLink" href="/II_Kings.19.24" data-ref="II Kings 19:24"&gt;2 Kings 19:24&lt;/a&gt;): “I have dug (קרתי)”; (&lt;a class ="refLink" href="/Isaiah.51.1" data-ref="Isaiah 51:1"&gt;Isaiah 51:1&lt;/a&gt;): “The hole of the pit from which you were dug out  (נקרתם); (&lt;a class ="refLink" href="/Proverbs.30.17" data-ref="Proverbs 30:17"&gt;Proverbs 30:17&lt;/a&gt;) “The ravens of the valley shall dig it out (יקרהו)". In O. F. forer.', 'כל בני שת ALL THE CHILDREN OF SETH — i.e., all nations, because all of them issued from Seth, the son of Adam, the first man (cf. Onkelos).'</t>
+  </si>
+  <si>
+    <t>'&lt;b&gt;He was oppressed, and he was afflicted&lt;/b&gt; Behold he was oppressed by taskmasters and people who exert pressure.', '&lt;b&gt;and he was afflicted&lt;/b&gt; with verbal taunts, sorparlec in O.F.', '&lt;b&gt;yet he would not open his mouth&lt;/b&gt; He would suffer and remain silent like the lamb that is brought to the slaughter, and like the ewe that is mute before her shearers.', '&lt;b&gt;and he would not open his mouth&lt;/b&gt; This refers to the lamb brought to the slaughter.'</t>
+  </si>
+  <si>
     <t>'&lt;b&gt;And he gave his grave to the wicked&lt;/b&gt; He subjected himself to be buried according to anything the wicked of the heathens (nations [mss., K’li Paz]) would decree upon him, for they would penalize him with death and the burial of donkeys in the intestines of the dogs.', '&lt;b&gt;to the wicked&lt;/b&gt; According to the will of the wicked, he was willing to be buried, and he would not deny the living God.', '&lt;b&gt;and to the wealthy with his kinds of death&lt;/b&gt; and to the will of the ruler he subjected himself to all kinds of death that he decreed upon him, because he did not wish to agree to (denial) [of the Torah] to commit evil and to rob like all the heathens (nations [mss., K’li Paz]) among whom he lived.', '&lt;b&gt;and there was no deceit in his mouth&lt;/b&gt; to accept idolatry (to accept a pagan deity as God [Parshandatha]).'</t>
   </si>
   <si>
+    <t>'&lt;b&gt;new heavens&lt;/b&gt; The princes above shall be renewed, and the princes of Israel shall be the upper princes and the princes of the heathens (the nations [Parshandatha]) will be lower, and so on the earth. ([K’li Paz reads:] The princes above shall be renewed, to raise up the humble and to humble the high ones, and so on the earth.) And some say that there will actually be new heavens, and that is correct, for Scripture proves it (infra 66:22): “For as the new heavens, etc.”'</t>
+  </si>
+  <si>
     <t>'&lt;b&gt;Seventy weeks [of years] have been decreed&lt;/b&gt; on Jerusalem from the day of the first destruction in the days of Zedekiah until it will be [destroyed] the second time.', '&lt;b&gt;to terminate the transgression and to end sin&lt;/b&gt; so that Israel should receive their complete retribution in the exile of Titus and his subjugation, in order that their transgressions should terminate, their sins should end, and their iniquities should be expiated, in order to bring upon them eternal righteousness and to anoint upon them (sic) the Holy of Holies: the Ark, the altars, and the holy vessels, which they will bring to them through the king Messiah. The number of seven weeks is four hundred and ninety years. The Babylonian exile was seventy [years] and the Second Temple stood four hundred and twenty [years].'</t>
   </si>
   <si>
-    <t>'&lt;b&gt;new heavens&lt;/b&gt; The princes above shall be renewed, and the princes of Israel shall be the upper princes and the princes of the heathens (the nations [Parshandatha]) will be lower, and so on the earth. ([K’li Paz reads:] The princes above shall be renewed, to raise up the humble and to humble the high ones, and so on the earth.) And some say that there will actually be new heavens, and that is correct, for Scripture proves it (infra 66:22): “For as the new heavens, etc.”'</t>
-  </si>
-  <si>
-    <t>'אראנו I SEE HIM — I see the preeminence of Jacob and his greatness, but it is not now (ולא עתה), but will be after some time.', 'דרך כוכב A STAR COMETH OUT [OF JACOB] — Understand this as the Targum does (“a king will arise from Jacob”). The word דרך has the same meaning as in (&lt;a class ="refLink" href="/Lamentations.2.4" data-ref="Lamentations 2:4"&gt;Lamentations 2:4&lt;/a&gt;): “He has bent (דרך lit., trodden) his bow; this expression is used because the star shoots across [the heavens] as an arrow does when the bow is trodden. In O. F. destent. It is as much as to say, “Prosperity (a good fortune) will rise”.', 'וקם שבט AND A שבט RISES [OUT OF ISRAEL] — a king, who chastises with the rod (שבט) and has sovereign power.', 'ומחץ פאתי מואב AND PIERCETH THE CORNERS OF MOAB — This is a reference to David of whom it is stated, (&lt;a class ="refLink" href="/II_Samuel.8.2" data-ref="II Samuel 8:2"&gt;II Samuel 8:2&lt;/a&gt;) “[And he smote Moab] … making them to lie down on the ground and he measured two lines to put to death etc.”.', 'וקרקר AND UNDERMINETH — This is an expression denoting “digging”, as in (&lt;a class ="refLink" href="/II_Kings.19.24" data-ref="II Kings 19:24"&gt;2 Kings 19:24&lt;/a&gt;): “I have dug (קרתי)”; (&lt;a class ="refLink" href="/Isaiah.51.1" data-ref="Isaiah 51:1"&gt;Isaiah 51:1&lt;/a&gt;): “The hole of the pit from which you were dug out  (נקרתם); (&lt;a class ="refLink" href="/Proverbs.30.17" data-ref="Proverbs 30:17"&gt;Proverbs 30:17&lt;/a&gt;) “The ravens of the valley shall dig it out (יקרהו)". In O. F. forer.', 'כל בני שת ALL THE CHILDREN OF SETH — i.e., all nations, because all of them issued from Seth, the son of Adam, the first man (cf. Onkelos).'</t>
-  </si>
-  <si>
     <t>' תמים PERFECT i. e. without blemish (&lt;a class ="refLink" href="/Mekhilta_d\'Rabbi_Yishmael.13.5.1" data-ref="Mekhilta d\'Rabbi Yishmael 13:5:1"&gt;Mekhilta d\'Rabbi Yishmael 13:5:1&lt;/a&gt;).', " בן שנה OF THE FIRST YEAR — the whole of its first year it is termed שנה בן, as much as to say, that it was born during this year (it does not mean that it is one year old — in its second year) (cf.Mekhilta d'Rabbi Yishmael 13:5:2).", ' מן הכבשים ומן העזים — i. e. either from these (a lamb) or from these (a goat) (i. e. the ו of ומן does not signify “and”, but “or”); for a goat, also, is called שה, as it is said, (&lt;a class ="refLink" href="/Deuteronomy.14.4" data-ref="Deuteronomy 14:4"&gt;Deuteronomy 14:4&lt;/a&gt;) “the שה of the goats” (שה means the young animal, either of the sheep or of the goats) (cf. &lt;a class ="refLink" href="/Mekhilta_d\'Rabbi_Yishmael.13.5.1" data-ref="Mekhilta d\'Rabbi Yishmael 13:5:1"&gt;Mekhilta d\'Rabbi Yishmael 13:5:1&lt;/a&gt;).'</t>
   </si>
   <si>
-    <t>'&lt;b&gt;He was oppressed, and he was afflicted&lt;/b&gt; Behold he was oppressed by taskmasters and people who exert pressure.', '&lt;b&gt;and he was afflicted&lt;/b&gt; with verbal taunts, sorparlec in O.F.', '&lt;b&gt;yet he would not open his mouth&lt;/b&gt; He would suffer and remain silent like the lamb that is brought to the slaughter, and like the ewe that is mute before her shearers.', '&lt;b&gt;and he would not open his mouth&lt;/b&gt; This refers to the lamb brought to the slaughter.'</t>
+    <t>['THERE SHALL STEP FORTH A STAR OUT OF JACOB. Because the Messiah will gather together the dispersed of Israel from all the corners of the earth, Balaam compares him [metaphorically] to &lt;i&gt;a star&lt;/i&gt; that passes through the firmament from the ends of heaven, just as it is said about [the Messiah]: &lt;i&gt;and behold, there came with the clouds of heaven, one like unto a son of man&lt;/i&gt; etc.&lt;sup class="footnote-marker"&gt;246&lt;/sup&gt;&lt;i class="footnote"&gt;Daniel 7:13.&lt;/i&gt; Balaam thus said that he saw that at a distant time &lt;i&gt;a star&lt;/i&gt; would pass from the ends of heaven, and there would rise out of it the sceptre of a ruler, &lt;i&gt;and he shall smite through the corners of Moab, and break down all the sons of Seth&lt;/i&gt;, the son of Adam,&lt;sup class="footnote-marker"&gt;247&lt;/sup&gt;&lt;i class="footnote"&gt;Genesis 5:3.&lt;/i&gt; who was the father of all the nations.&lt;sup class="footnote-marker"&gt;248&lt;/sup&gt;&lt;i class="footnote"&gt;See Ramban &lt;i&gt;ibid.&lt;/i&gt;, Vol. I, p. 98.&lt;/i&gt; He mentioned &lt;i&gt;the corners of Moab&lt;/i&gt; in order to inform Balak that his people would not fall into the hand of Israel now, but &lt;i&gt;in the end of days&lt;/i&gt;&lt;sup class="footnote-marker"&gt;239&lt;/sup&gt;&lt;i class="footnote"&gt;Verse 14.&lt;/i&gt; Moab will not be saved from the hand of the ruling king [in Israel]. And the meaning of &lt;i&gt;‘the corners’ of Moab&lt;/i&gt; is that this ruler [in Israel] &lt;i&gt;will break down all the sons of Seth&lt;/i&gt;, and they [Moab] will not be saved, even though they are &lt;i&gt;cut off on ‘the corner,’&lt;/i&gt;&lt;sup class="footnote-marker"&gt;249&lt;/sup&gt;&lt;i class="footnote"&gt;Jeremiah 9:25. This is an epithet for certain Arabian tribes, who had the corners of their hair clipped. Ramban here uses this term metaphorically, in its literal sense of “cut off in the corner”, to refer to a people who live in the remotest corners of the world.&lt;/i&gt; and have no name among the nations, and will not fight against Israel.']</t>
   </si>
   <si>
     <t>['TAKE NOW THY SON, THINE ONLY SON. Since Isaac was the son of the mistress and he alone was to be the one to carry his name, He called him Abraham’s only son. The description was for the purpose of magnifying the command, thus saying: “Take now thy only son, the beloved one, Isaac, and bring him up before Me as a burnt-offering.”', 'MORIAH. Rashi comments: “This is Jerusalem, and we find it in the book of Chronicles: &lt;i&gt;To build the house of the Eternal at Jerusalem on mount Moriah&lt;/i&gt;.&lt;sup class="footnote-marker"&gt;366&lt;/sup&gt;&lt;i class="footnote"&gt;II Chronicles 3:1.&lt;/i&gt; Our Rabbis have explained that it is called &lt;i&gt;Moriah&lt;/i&gt; (instruction) because from the Temple built there on that mountain, instruction came forth to Israel.&lt;sup class="footnote-marker"&gt;367&lt;/sup&gt;&lt;i class="footnote"&gt;The Chamber of Hewn Stone (&lt;i&gt;Lishchat hagazith&lt;/i&gt;), the seat of the Great Sanhedrin, which was the highest court in Israel, was located in the Court of the Temple. See &lt;a class ="refLink" href="/Deuteronomy.17.8-11" data-ref="Deuteronomy 17:8-11"&gt;Deuteronomy 17:8-11&lt;/a&gt;.&lt;/i&gt; Onkelos translated it as “the land of Worship.” This he derived on the basis of reference to the burning of incense, which contained &lt;i&gt;mor&lt;/i&gt;&lt;sup class="footnote-marker"&gt;368&lt;/sup&gt;&lt;i class="footnote"&gt;Hence the name &lt;i&gt;Moriah&lt;/i&gt;: the mountain on which &lt;i&gt;mor&lt;/i&gt; (myrrh), as part of the incense, was to be burnt. Thus according to Rashi’s understanding of Onkelos. Ramban will later differ with this interpretation in the meaning of Onkelos.&lt;/i&gt; (myrrh) and other spices, [as part of the Divine Service].”&lt;br&gt;Now if so, [i.e., if this be the explanation of the name &lt;i&gt;Moriah&lt;/i&gt;], the meaning of the verse will then be, “Go into the land which will be called &lt;i&gt;Moriah&lt;/i&gt;.” Or it may be that it was always called so on account of the future. In Bereshith Rabbah,&lt;sup class="footnote-marker"&gt;369&lt;/sup&gt;&lt;i class="footnote"&gt;55:9.&lt;/i&gt; the Sages have said thus: “The Rabbis say, &lt;i&gt;Go into the land of Moriah&lt;/i&gt; means into the land where incense will be offered on the altar of G-d, even as it is said, &lt;i&gt;I will get me to the mountain ‘hamor’ (of myrrh)&lt;/i&gt;.”&lt;sup class="footnote-marker"&gt;370&lt;/sup&gt;&lt;i class="footnote"&gt;Song of Songs 4:6.&lt;/i&gt; But the opinion of Onkelos, who said “the land of worship,” does not appear to be based on the myrrh in the incense, as Rashi said, for the word “service” does not refer to one of the species used in one of the Divine Services. Besides, why did not Onkelos say, “to the land of the incense of spices?” Instead, Onkelos’ intent is to say, “in the land in which they will worhip G-d.”&lt;br&gt;Onkelos thus matched that which the Sages interpreted in Pirkei d’Rabbi Eliezer, where they said,&lt;sup class="footnote-marker"&gt;371&lt;/sup&gt;&lt;i class="footnote"&gt;Chapter 31.&lt;/i&gt; “The Holy One, blessed be He, showed Abraham the altar with a finger. He said to him, ‘This is the altar on which the first man sacrificed. This is the altar on which Cain and Abel sacrificed. This is the altar on which Noah and his sons sacrificed.’ For it is said, &lt;i&gt;And Abraham built ‘hamizbei’ach’ (the altar) there&lt;/i&gt;,&lt;sup class="footnote-marker"&gt;372&lt;/sup&gt;&lt;i class="footnote"&gt;Verse 9 here.&lt;/i&gt; &lt;i&gt;mizbei’ach&lt;/i&gt; (an altar) is not written here, rather, &lt;i&gt;hamizbei’ach (the&lt;/i&gt; altar). This is the altar on which the predecessors have sacrificed.” Thus far [is the interpretation of Pirkei d’Rabbi Eliezer]. And the name &lt;i&gt;Moriah&lt;/i&gt; the Rabbis derived from the word &lt;i&gt;mora&lt;/i&gt; (fear), for there the people feared G-d and worshipped Him.&lt;br&gt;The correct interpretation, in line with the plain meaning of Scripture, is that the name &lt;i&gt;Moriah&lt;/i&gt; is like the expression, &lt;i&gt;To the mountain of myrrh, and to the hill of frankincense&lt;/i&gt;,&lt;sup class="footnote-marker"&gt;370&lt;/sup&gt;&lt;i class="footnote"&gt;Song of Songs 4:6.&lt;/i&gt; for on that mountain [Moriah] are found &lt;i&gt;myrrh, aloes, and cinnamon&lt;/i&gt;,&lt;sup class="footnote-marker"&gt;373&lt;/sup&gt;&lt;i class="footnote"&gt;Proverbs 7:17.&lt;/i&gt; even as the Rabbis have said:&lt;sup class="footnote-marker"&gt;374&lt;/sup&gt;&lt;i class="footnote"&gt;Yerushalmi &lt;a class ="refLink" href="/Mishnah_Peah.7.3" data-ref="Mishnah Peah 7:3"&gt;Peah 7:3&lt;/a&gt;.&lt;/i&gt; “Cinnamon grew in the Land of Israel, and goats and deers ate of it.” Or it may be that it was so called in praise of the Land of Israel.&lt;sup class="footnote-marker"&gt;375&lt;/sup&gt;&lt;i class="footnote"&gt;But myrrh, aloes and cinnamon actually do not grow on mount Moriah itself. It was, however, called by that name, in order to give praise to the land where these things grow.&lt;/i&gt;&lt;br&gt;Now here Scripture calls the name of the land, &lt;i&gt;the land of Moriah&lt;/i&gt;, and there [in the book of Chronicles, mentioned above],&lt;sup class="footnote-marker"&gt;366&lt;/sup&gt;&lt;i class="footnote"&gt;II Chronicles 3:1.&lt;/i&gt; it appears that only the Temple mount was called mount Moriah. Perhaps, the city&lt;sup class="footnote-marker"&gt;376&lt;/sup&gt;&lt;i class="footnote"&gt;“The City.” The Tur, quoting Ramban, has “the land.”&lt;/i&gt; was called by the name of that mountain which it contains, [and the name “land of Moriah” means] the land which contains the &lt;i&gt;Moriah&lt;/i&gt;, but it was the mountain alone that was called &lt;i&gt;Moriah&lt;/i&gt;. Now Abraham knew the land but did not know the mountain. Hence G-d told him to go to the land of &lt;i&gt;Moriah&lt;/i&gt;, and He will there show him one of the mountains which is called by that name. He commanded him to offer up his son in that place for that is &lt;i&gt;the mountain which G-d hath desired for His abode&lt;/i&gt;,&lt;sup class="footnote-marker"&gt;377&lt;/sup&gt;&lt;i class="footnote"&gt;Psalms 68:17.&lt;/i&gt; and He wanted the merit of the &lt;i&gt;Akeidah&lt;/i&gt; (the Binding of Isaac) to be in the sacrifices forever, as Abraham said, &lt;i&gt;The Eternal seeth&lt;/i&gt;.&lt;sup class="footnote-marker"&gt;378&lt;/sup&gt;&lt;i class="footnote"&gt;Verse 14 here.&lt;/i&gt; Moreover, &lt;i&gt;for His righteousness’ sake&lt;/i&gt;,&lt;sup class="footnote-marker"&gt;379&lt;/sup&gt;&lt;i class="footnote"&gt;Isaiah 42:21.&lt;/i&gt; He increased the scope of the trial and wanted Abraham to do it after walking three days. Had Abraham been commanded to do so suddenly at his place, his deed would have been performed in haste and confusion, but since it was done after walking for days it was thus performed with reflection of mind and counsel. And so did the Rabbis say in Bereshith Rabbah:&lt;sup class="footnote-marker"&gt;380&lt;/sup&gt;&lt;i class="footnote"&gt;55:5.&lt;/i&gt; “Rabbi Akiba said, ‘G-d surely tried [Abraham with a clear-cut situation] so that people should not say that He confounded him and confused him and he did not know what to do.’”']</t>
   </si>
   <si>
-    <t>['THERE SHALL STEP FORTH A STAR OUT OF JACOB. Because the Messiah will gather together the dispersed of Israel from all the corners of the earth, Balaam compares him [metaphorically] to &lt;i&gt;a star&lt;/i&gt; that passes through the firmament from the ends of heaven, just as it is said about [the Messiah]: &lt;i&gt;and behold, there came with the clouds of heaven, one like unto a son of man&lt;/i&gt; etc.&lt;sup class="footnote-marker"&gt;246&lt;/sup&gt;&lt;i class="footnote"&gt;Daniel 7:13.&lt;/i&gt; Balaam thus said that he saw that at a distant time &lt;i&gt;a star&lt;/i&gt; would pass from the ends of heaven, and there would rise out of it the sceptre of a ruler, &lt;i&gt;and he shall smite through the corners of Moab, and break down all the sons of Seth&lt;/i&gt;, the son of Adam,&lt;sup class="footnote-marker"&gt;247&lt;/sup&gt;&lt;i class="footnote"&gt;Genesis 5:3.&lt;/i&gt; who was the father of all the nations.&lt;sup class="footnote-marker"&gt;248&lt;/sup&gt;&lt;i class="footnote"&gt;See Ramban &lt;i&gt;ibid.&lt;/i&gt;, Vol. I, p. 98.&lt;/i&gt; He mentioned &lt;i&gt;the corners of Moab&lt;/i&gt; in order to inform Balak that his people would not fall into the hand of Israel now, but &lt;i&gt;in the end of days&lt;/i&gt;&lt;sup class="footnote-marker"&gt;239&lt;/sup&gt;&lt;i class="footnote"&gt;Verse 14.&lt;/i&gt; Moab will not be saved from the hand of the ruling king [in Israel]. And the meaning of &lt;i&gt;‘the corners’ of Moab&lt;/i&gt; is that this ruler [in Israel] &lt;i&gt;will break down all the sons of Seth&lt;/i&gt;, and they [Moab] will not be saved, even though they are &lt;i&gt;cut off on ‘the corner,’&lt;/i&gt;&lt;sup class="footnote-marker"&gt;249&lt;/sup&gt;&lt;i class="footnote"&gt;Jeremiah 9:25. This is an epithet for certain Arabian tribes, who had the corners of their hair clipped. Ramban here uses this term metaphorically, in its literal sense of “cut off in the corner”, to refer to a people who live in the remotest corners of the world.&lt;/i&gt; and have no name among the nations, and will not fight against Israel.']</t>
-  </si>
-  <si>
     <t>['כל אשר בו מום לא תקריבו כי לא לרצון יהיה לכם, as elaborated on by Maleachi 1,8.\n']</t>
   </si>
   <si>
@@ -191,6 +197,36 @@
   </si>
   <si>
     <t>['אראנו, I can clearly see it but it is not due now.', 'דרך כוכב, both physical and enduring. We find the word כוכב used in this sense in &lt;a class ="refLink" href="/Daniel.12.3" data-ref="Daniel 12:3"&gt;Daniel 12,3&lt;/a&gt; as ומצדיקי הרבים ככוכבם לעולם, “and those who lead many to righteousness will be like the stars forever and ever.”', 'ומחץ פאתי מואב, even though all the nations will be wiped out by G’d the nations Edom and Moav will be decisively defeated by the Jewish people themselves as an act of vengeance for their longstanding enmity to the Jewish people.\n']</t>
+  </si>
+  <si>
+    <t>Anything that has a blemish on it you shall not bring, for it will not be accepted favorably for you.</t>
+  </si>
+  <si>
+    <t>But if you will not do this, behold, you will have sinned against [&lt;b&gt;before&lt;/b&gt;] Adonoy and you must realize that your sin will find you!</t>
+  </si>
+  <si>
+    <t>I see it but not now, I perceive it but not in the near future; a star [&lt;b&gt;king&lt;/b&gt;] has gone forth from Yaakov, and a staff has arisen [&lt;b&gt;the Moshiach will be magnified by&lt;/b&gt;] from Yisroel, which will smash the corners [&lt;b&gt;kill the leaders&lt;/b&gt;] of Moav, and impale all of the sons of Sheis [&lt;b&gt;will rule over mankind&lt;/b&gt;].</t>
+  </si>
+  <si>
+    <t>He said, Please [&lt;b&gt;Now&lt;/b&gt;] take your son, your only one, who you love—Yitzchok—and go to the land of Moriah [&lt;b&gt;worship&lt;/b&gt;]. Sacrifice him [&lt;b&gt;before me&lt;/b&gt;] as a burnt-offering on one of the mountains which I will designate to you.</t>
+  </si>
+  <si>
+    <t>A flawless lamb, a yearling male must be in your possession. You may take it from sheep or goats.</t>
+  </si>
+  <si>
+    <t>But anything that hath a blemish you shall not offer; for that will not be acceptable from you.</t>
+  </si>
+  <si>
+    <t>But if you will not perform this, behold, ye will have sinned before the Lord your God, and know that your sin will meet you.</t>
+  </si>
+  <si>
+    <t>I shall see Him, but not now; I shall behold Him, but it is not near. When the mighty King of Jakob's house shall reign, and the Meshiha, the Power-sceptre of Israel, be anointed, He will slay the princes of the Moabaee, and bring to nothing all the children of Sheth, the armies of Gog who will do battle against Israel and all their carcases shall fall before Him.</t>
+  </si>
+  <si>
+    <t>And He said, Take now thy son, thy only one whom thou lovest, Izhak, and go into the land of worship, and offer him there, a whole burnt offering, upon one of the mountains that I will tell thee.</t>
+  </si>
+  <si>
+    <t>The lamb shall be perfect, a male, the son of a year he shall be to you; from the sheep or from the young goats ye may take.</t>
   </si>
 </sst>
 </file>
@@ -548,13 +584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,68 +618,77 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
         <v>22</v>
       </c>
-      <c r="C2">
+      <c r="C4">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>42</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>32</v>
-      </c>
-      <c r="C4">
-        <v>23</v>
-      </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>58</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -654,75 +699,96 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>26</v>
-      </c>
-      <c r="C7">
-        <v>11</v>
-      </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>22</v>
@@ -731,136 +797,142 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>53</v>
+      </c>
+      <c r="C12">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>33</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>65</v>
-      </c>
-      <c r="C12">
-        <v>17</v>
-      </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
         <v>55</v>
       </c>
-      <c r="H13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>53</v>
-      </c>
-      <c r="C15">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" t="s">
-        <v>53</v>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>